<commit_message>
Enable maps for dwellings, income and access.
</commit_message>
<xml_diff>
--- a/visualizer_2/SILOVisualizer/visualizerMenuOptions.xlsx
+++ b/visualizer_2/SILOVisualizer/visualizerMenuOptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c8722396f3f1ac9b/11_Nuevos_proyectos/MSM/msmvisualizer/visualizer_2/SILOVisualizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="13_ncr:40009_{7BB1EE10-1CE9-4AF2-87FB-8573E066B90B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{D9C9272C-863C-4388-865E-B2F0C7CA9256}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="13_ncr:40009_{7BB1EE10-1CE9-4AF2-87FB-8573E066B90B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7DA1A9E5-2090-438B-A784-454EB1CF8B45}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26070" yWindow="2730" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="menu" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="120">
   <si>
     <t>visualization</t>
   </si>
@@ -369,6 +369,18 @@
   </si>
   <si>
     <t>examples/muc/av0/resultFileSpatial_2.csv</t>
+  </si>
+  <si>
+    <t>Auto_accessibility</t>
+  </si>
+  <si>
+    <t>Transit_accessibility</t>
+  </si>
+  <si>
+    <t>autoAccessibility</t>
+  </si>
+  <si>
+    <t>transitAccessibility</t>
   </si>
 </sst>
 </file>
@@ -1209,10 +1221,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,6 +1446,12 @@
       <c r="C12" t="s">
         <v>22</v>
       </c>
+      <c r="D12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12" t="s">
+        <v>118</v>
+      </c>
       <c r="G12" t="s">
         <v>83</v>
       </c>
@@ -1443,16 +1461,16 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>117</v>
       </c>
       <c r="E13" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="G13" t="s">
         <v>83</v>
@@ -1469,10 +1487,10 @@
         <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G14" t="s">
         <v>83</v>
@@ -1489,10 +1507,10 @@
         <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G15" t="s">
         <v>83</v>
@@ -1509,10 +1527,10 @@
         <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G16" t="s">
         <v>83</v>
@@ -1520,13 +1538,19 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" t="s">
+        <v>97</v>
       </c>
       <c r="G17" t="s">
         <v>83</v>
@@ -1537,16 +1561,10 @@
         <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G18" t="s">
         <v>83</v>
@@ -1563,10 +1581,10 @@
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G19" t="s">
         <v>83</v>
@@ -1583,10 +1601,10 @@
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G20" t="s">
         <v>83</v>
@@ -1603,10 +1621,10 @@
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G21" t="s">
         <v>83</v>
@@ -1623,10 +1641,10 @@
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G22" t="s">
         <v>83</v>
@@ -1643,10 +1661,10 @@
         <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G23" t="s">
         <v>83</v>
@@ -1663,10 +1681,10 @@
         <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G24" t="s">
         <v>83</v>
@@ -1683,10 +1701,10 @@
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G25" t="s">
         <v>83</v>
@@ -1697,16 +1715,16 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G26" t="s">
         <v>83</v>
@@ -1723,10 +1741,10 @@
         <v>49</v>
       </c>
       <c r="D27" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G27" t="s">
         <v>83</v>
@@ -1743,10 +1761,10 @@
         <v>49</v>
       </c>
       <c r="D28" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="E28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G28" t="s">
         <v>83</v>
@@ -1763,10 +1781,10 @@
         <v>49</v>
       </c>
       <c r="D29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G29" t="s">
         <v>83</v>
@@ -1777,16 +1795,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="D30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G30" t="s">
         <v>83</v>
@@ -1803,10 +1821,10 @@
         <v>18</v>
       </c>
       <c r="D31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G31" t="s">
         <v>83</v>
@@ -1823,10 +1841,10 @@
         <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G32" t="s">
         <v>83</v>
@@ -1843,10 +1861,10 @@
         <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G33" t="s">
         <v>83</v>
@@ -1857,16 +1875,16 @@
         <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="C34" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E34" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G34" t="s">
         <v>83</v>
@@ -1883,10 +1901,10 @@
         <v>66</v>
       </c>
       <c r="D35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E35" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G35" t="s">
         <v>83</v>
@@ -1903,10 +1921,10 @@
         <v>66</v>
       </c>
       <c r="D36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G36" t="s">
         <v>83</v>
@@ -1923,10 +1941,10 @@
         <v>66</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G37" t="s">
         <v>83</v>
@@ -1937,16 +1955,16 @@
         <v>29</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D38" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E38" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G38" t="s">
         <v>83</v>
@@ -1963,10 +1981,10 @@
         <v>76</v>
       </c>
       <c r="D39" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E39" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G39" t="s">
         <v>83</v>
@@ -1983,12 +2001,32 @@
         <v>76</v>
       </c>
       <c r="D40" t="s">
+        <v>79</v>
+      </c>
+      <c r="E40" t="s">
+        <v>80</v>
+      </c>
+      <c r="G40" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" t="s">
         <v>81</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E41" t="s">
         <v>82</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G41" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2001,8 +2039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Organize and create example inputs in Kagawa implementation
</commit_message>
<xml_diff>
--- a/visualizer_2/SILOVisualizer/visualizerMenuOptions.xlsx
+++ b/visualizer_2/SILOVisualizer/visualizerMenuOptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c8722396f3f1ac9b/11_Nuevos_proyectos/MSM/msmvisualizer/visualizer_2/SILOVisualizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="114_{3DC57B6D-9755-4C51-B800-D479A9349C62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{876F8294-31A4-4297-8B04-561847882A38}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="114_{3DC57B6D-9755-4C51-B800-D479A9349C62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AEE842A1-5CF2-4CE5-943A-4D64B0EC559B}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="menu" sheetId="1" r:id="rId1"/>
@@ -2034,7 +2034,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C9" sqref="B9:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Inputs for dynamic menu
</commit_message>
<xml_diff>
--- a/visualizer_2/SILOVisualizer/visualizerMenuOptions.xlsx
+++ b/visualizer_2/SILOVisualizer/visualizerMenuOptions.xlsx
@@ -1,27 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c8722396f3f1ac9b/11_Nuevos_proyectos/MSM/msmvisualizer/visualizer_2/SILOVisualizer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="114_{3DC57B6D-9755-4C51-B800-D479A9349C62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AEE842A1-5CF2-4CE5-943A-4D64B0EC559B}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="114_{3DC57B6D-9755-4C51-B800-D479A9349C62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3C58EF84-C503-4900-BB63-90356A87B52F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="menu" sheetId="1" r:id="rId1"/>
     <sheet name="config" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">menu!$A$1:$I$46</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="138">
   <si>
     <t>visualization</t>
   </si>
@@ -236,12 +239,6 @@
     <t>reAvailableLand</t>
   </si>
   <si>
-    <t>Jobs by sector and region</t>
-  </si>
-  <si>
-    <t>reJobsSect</t>
-  </si>
-  <si>
     <t>Total Jobs</t>
   </si>
   <si>
@@ -272,9 +269,6 @@
     <t>dwellEvents</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>avaiLand</t>
   </si>
   <si>
@@ -375,6 +369,75 @@
   </si>
   <si>
     <t>hhInc_.60000</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>Dwelling</t>
+  </si>
+  <si>
+    <t>resultFileSpatial.csv</t>
+  </si>
+  <si>
+    <t>required_file_1</t>
+  </si>
+  <si>
+    <t>required_file_2</t>
+  </si>
+  <si>
+    <t>required_file_3</t>
+  </si>
+  <si>
+    <t>popyear.csv</t>
+  </si>
+  <si>
+    <t>dwellings.csv</t>
+  </si>
+  <si>
+    <t>hhSize.csv</t>
+  </si>
+  <si>
+    <t>hhType.csv</t>
+  </si>
+  <si>
+    <t>aveHhSize.csv</t>
+  </si>
+  <si>
+    <t>hhAveIncome.csv</t>
+  </si>
+  <si>
+    <t>carOwnership.csv</t>
+  </si>
+  <si>
+    <t>hhRentAndIncome.csv</t>
+  </si>
+  <si>
+    <t>popYear.csv</t>
+  </si>
+  <si>
+    <t>persByRace.csv</t>
+  </si>
+  <si>
+    <t>labourParticipationRate.csv</t>
+  </si>
+  <si>
+    <t>persMigrants.csv</t>
+  </si>
+  <si>
+    <t>dwellingQualityLevel.csv</t>
+  </si>
+  <si>
+    <t>commutingDistance.csv</t>
+  </si>
+  <si>
+    <t>jobsBySectorAndRegion.csv</t>
+  </si>
+  <si>
+    <t>eventCounts.csv</t>
   </si>
 </sst>
 </file>
@@ -698,7 +761,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -813,6 +876,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -858,8 +936,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1215,816 +1294,1066 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H41"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:G41"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="7" max="9" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C31" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C32" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
-        <v>91</v>
-      </c>
-      <c r="E8" t="s">
-        <v>87</v>
-      </c>
-      <c r="G8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="D32" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E9" t="s">
-        <v>88</v>
-      </c>
-      <c r="G9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="D33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C34" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E10" t="s">
-        <v>89</v>
-      </c>
-      <c r="G10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E11" t="s">
-        <v>90</v>
-      </c>
-      <c r="G11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" t="s">
-        <v>110</v>
-      </c>
-      <c r="E12" t="s">
-        <v>112</v>
-      </c>
-      <c r="G12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" t="s">
-        <v>113</v>
-      </c>
-      <c r="G13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" t="s">
-        <v>114</v>
-      </c>
-      <c r="G14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="C45" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" t="s">
-        <v>117</v>
-      </c>
-      <c r="G17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" t="s">
-        <v>31</v>
-      </c>
-      <c r="G18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" t="s">
-        <v>41</v>
-      </c>
-      <c r="G23" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G24" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" t="s">
-        <v>45</v>
-      </c>
-      <c r="G25" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" t="s">
-        <v>47</v>
-      </c>
-      <c r="G26" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" t="s">
-        <v>50</v>
-      </c>
-      <c r="E27" t="s">
-        <v>51</v>
-      </c>
-      <c r="G27" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" t="s">
-        <v>52</v>
-      </c>
-      <c r="G28" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" t="s">
-        <v>53</v>
-      </c>
-      <c r="E29" t="s">
-        <v>54</v>
-      </c>
-      <c r="G29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" t="s">
-        <v>55</v>
-      </c>
-      <c r="E30" t="s">
-        <v>56</v>
-      </c>
-      <c r="G30" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" t="s">
-        <v>57</v>
-      </c>
-      <c r="E31" t="s">
-        <v>58</v>
-      </c>
-      <c r="G31" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32" t="s">
-        <v>59</v>
-      </c>
-      <c r="E32" t="s">
-        <v>60</v>
-      </c>
-      <c r="G32" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" t="s">
-        <v>61</v>
-      </c>
-      <c r="E33" t="s">
-        <v>62</v>
-      </c>
-      <c r="G33" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>29</v>
-      </c>
-      <c r="B34" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" t="s">
-        <v>63</v>
-      </c>
-      <c r="E34" t="s">
-        <v>64</v>
-      </c>
-      <c r="G34" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="D45" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C35" t="s">
+      <c r="E45" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D35" t="s">
-        <v>67</v>
-      </c>
-      <c r="E35" t="s">
-        <v>68</v>
-      </c>
-      <c r="G35" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" t="s">
-        <v>66</v>
-      </c>
-      <c r="D36" t="s">
-        <v>69</v>
-      </c>
-      <c r="E36" t="s">
-        <v>70</v>
-      </c>
-      <c r="G36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>29</v>
-      </c>
-      <c r="B37" t="s">
-        <v>65</v>
-      </c>
-      <c r="C37" t="s">
-        <v>66</v>
-      </c>
-      <c r="D37" t="s">
-        <v>71</v>
-      </c>
-      <c r="E37" t="s">
-        <v>72</v>
-      </c>
-      <c r="G37" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" t="s">
-        <v>65</v>
-      </c>
-      <c r="C38" t="s">
-        <v>66</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E46" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G38" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" t="s">
-        <v>76</v>
-      </c>
-      <c r="D39" t="s">
-        <v>77</v>
-      </c>
-      <c r="E39" t="s">
-        <v>78</v>
-      </c>
-      <c r="G39" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" t="s">
-        <v>75</v>
-      </c>
-      <c r="C40" t="s">
-        <v>76</v>
-      </c>
-      <c r="D40" t="s">
-        <v>79</v>
-      </c>
-      <c r="E40" t="s">
-        <v>80</v>
-      </c>
-      <c r="G40" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>29</v>
-      </c>
-      <c r="B41" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" t="s">
-        <v>76</v>
-      </c>
-      <c r="D41" t="s">
-        <v>81</v>
-      </c>
-      <c r="E41" t="s">
-        <v>82</v>
-      </c>
-      <c r="G41" t="s">
-        <v>83</v>
-      </c>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I46" xr:uid="{C87CD6B2-9C22-437D-80D9-30BD4E3364FE}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="aspatial"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2033,7 +2362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="B9:C10"/>
     </sheetView>
   </sheetViews>
@@ -2046,13 +2375,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2060,7 +2389,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C2">
         <v>2011</v>
@@ -2071,7 +2400,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C3">
         <v>2050</v>
@@ -2082,18 +2411,18 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C5">
         <v>2000</v>
@@ -2101,10 +2430,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C6">
         <v>2005</v>
@@ -2112,21 +2441,21 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" t="s">
         <v>102</v>
-      </c>
-      <c r="B7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2134,7 +2463,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C9">
         <v>2010</v>
@@ -2145,7 +2474,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C10">
         <v>2050</v>
@@ -2156,18 +2485,18 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C12">
         <v>2011</v>
@@ -2175,10 +2504,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C13">
         <v>2040</v>
@@ -2186,29 +2515,29 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" t="s">
         <v>103</v>
-      </c>
-      <c r="B14" t="s">
-        <v>100</v>
-      </c>
-      <c r="C14" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -2216,10 +2545,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C17">
         <v>10</v>
@@ -2227,13 +2556,13 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C18" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to add the bkk use case
</commit_message>
<xml_diff>
--- a/visualizer_2/SILOVisualizer/visualizerMenuOptions.xlsx
+++ b/visualizer_2/SILOVisualizer/visualizerMenuOptions.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c8722396f3f1ac9b/11_Nuevos_proyectos/MSM/msmvisualizer/visualizer_2/SILOVisualizer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\msm-visualizer\visualizer_2\SILOVisualizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="114_{3DC57B6D-9755-4C51-B800-D479A9349C62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3C58EF84-C503-4900-BB63-90356A87B52F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="menu" sheetId="1" r:id="rId1"/>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="140">
   <si>
     <t>visualization</t>
   </si>
@@ -438,12 +437,18 @@
   </si>
   <si>
     <t>eventCounts.csv</t>
+  </si>
+  <si>
+    <t>map</t>
+  </si>
+  <si>
+    <t>bkk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1293,11 +1298,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
@@ -2347,7 +2352,7 @@
       <c r="I46" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I46" xr:uid="{C87CD6B2-9C22-437D-80D9-30BD4E3364FE}">
+  <autoFilter ref="A1:I46">
     <filterColumn colId="0">
       <filters>
         <filter val="aspatial"/>
@@ -2359,11 +2364,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="B9:C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2565,6 +2570,39 @@
         <v>105</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20">
+        <v>2115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" t="s">
+        <v>138</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>